<commit_message>
Change File Status read
</commit_message>
<xml_diff>
--- a/account.xlsx
+++ b/account.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\Works\LRHDT\ProjectSave\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66F12EC7-14DF-42E3-9BB6-BBECAD762D75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21E77240-0F1B-43DC-87A9-34895BC145DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="4">
   <si>
     <t>user2131200001</t>
   </si>
@@ -37,105 +37,6 @@
   </si>
   <si>
     <t>2131200001</t>
-  </si>
-  <si>
-    <t>user2131200002</t>
-  </si>
-  <si>
-    <t>admin1</t>
-  </si>
-  <si>
-    <t>2131200002</t>
-  </si>
-  <si>
-    <t>Cuong</t>
-  </si>
-  <si>
-    <t>12345</t>
-  </si>
-  <si>
-    <t>Le Chi Cuong</t>
-  </si>
-  <si>
-    <t>user2131200003</t>
-  </si>
-  <si>
-    <t>minh</t>
-  </si>
-  <si>
-    <t>Minh</t>
-  </si>
-  <si>
-    <t>2131200003</t>
-  </si>
-  <si>
-    <t>Minh123</t>
-  </si>
-  <si>
-    <t>123456</t>
-  </si>
-  <si>
-    <t>Dinh Tran Anh Minh</t>
-  </si>
-  <si>
-    <t>user213120001</t>
-  </si>
-  <si>
-    <t>cuong</t>
-  </si>
-  <si>
-    <t>213120001</t>
-  </si>
-  <si>
-    <t>user213120003</t>
-  </si>
-  <si>
-    <t>cuong1</t>
-  </si>
-  <si>
-    <t>213120003</t>
-  </si>
-  <si>
-    <t>user2131200010</t>
-  </si>
-  <si>
-    <t>han1</t>
-  </si>
-  <si>
-    <t>Han</t>
-  </si>
-  <si>
-    <t>2131200010</t>
-  </si>
-  <si>
-    <t>user21312000013</t>
-  </si>
-  <si>
-    <t>cuong123</t>
-  </si>
-  <si>
-    <t>21312000013</t>
-  </si>
-  <si>
-    <t>cuong1234</t>
-  </si>
-  <si>
-    <t>user21312000014</t>
-  </si>
-  <si>
-    <t>cuong12345</t>
-  </si>
-  <si>
-    <t>21312000014</t>
-  </si>
-  <si>
-    <t>user21312000010</t>
-  </si>
-  <si>
-    <t>21312000010</t>
-  </si>
-  <si>
-    <t>cuong12</t>
   </si>
 </sst>
 </file>
@@ -454,15 +355,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1">
       <c r="A1" t="s" s="0">
         <v>0</v>
       </c>
@@ -475,105 +376,13 @@
       <c r="D1" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="E1" s="0" t="n">
+      <c r="E1" t="n" s="0">
         <v>2021.0</v>
       </c>
       <c r="F1" t="s" s="0">
         <v>3</v>
       </c>
       <c r="G1" t="b" s="0">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" t="s" s="0">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s" s="0">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s" s="0">
-        <v>9</v>
-      </c>
-      <c r="E2" t="n" s="0">
-        <v>2021.0</v>
-      </c>
-      <c r="F2" t="s" s="0">
-        <v>6</v>
-      </c>
-      <c r="G2" t="b" s="0">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s" s="0">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s" s="0">
-        <v>14</v>
-      </c>
-      <c r="C3" t="s" s="0">
-        <v>15</v>
-      </c>
-      <c r="D3" t="s" s="0">
-        <v>16</v>
-      </c>
-      <c r="E3" t="n" s="0">
-        <v>2021.0</v>
-      </c>
-      <c r="F3" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="G3" t="b" s="0">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="B4" t="s" s="0">
-        <v>24</v>
-      </c>
-      <c r="C4" t="s" s="0">
-        <v>2</v>
-      </c>
-      <c r="D4" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="E4" t="n" s="0">
-        <v>2021.0</v>
-      </c>
-      <c r="F4" t="s" s="0">
-        <v>26</v>
-      </c>
-      <c r="G4" t="b" s="0">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s" s="0">
-        <v>34</v>
-      </c>
-      <c r="B5" t="s" s="0">
-        <v>28</v>
-      </c>
-      <c r="C5" t="s" s="0">
-        <v>2</v>
-      </c>
-      <c r="D5" t="s" s="0">
-        <v>9</v>
-      </c>
-      <c r="E5" t="n" s="0">
-        <v>2021.0</v>
-      </c>
-      <c r="F5" t="s" s="0">
-        <v>35</v>
-      </c>
-      <c r="G5" t="b" s="0">
         <v>1</v>
       </c>
     </row>

</xml_diff>